<commit_message>
Two new Diagnostic Report IG profiles have been added for pathology...
They are:
- Pathology Report (Composition)
- Order Details for Pathology Report (ServiceRequest)
Both are in an initial 'shell' state, with more details to follow.
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/patient-mhr-1.xlsx
+++ b/output/DiagnosticReport/patient-mhr-1.xlsx
@@ -6918,7 +6918,7 @@
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F43" t="s" s="2">
         <v>51</v>
@@ -7370,7 +7370,7 @@
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F47" t="s" s="2">
         <v>51</v>

</xml_diff>

<commit_message>
Diagnostic Report and Event Summary - completed My Health Record Patient
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/patient-mhr-1.xlsx
+++ b/output/DiagnosticReport/patient-mhr-1.xlsx
@@ -153,14 +153,14 @@
     <t/>
   </si>
   <si>
-    <t>A representation of a patient in the context of exchange of health information with the My Health Record system</t>
+    <t>A patient in the context of electronic exchange of health information</t>
   </si>
   <si>
     <t>Demographics and other administrative information about an individual receiving care or other health-related services.</t>
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}inv-pat-0:If there is a birth time its date shall be the birth date {birthDate.extension('http://hl7.org/fhir/StructureDefinition/patient-birthTime').exists() implies birthDate.extension('http://hl7.org/fhir/StructureDefinition/patient-birthTime').value.toString().substring(0,10) = birthDate.toString()}inv-dh-pat-01:One patient name shall have at least a family name {name.family.exists()}inv-dh-pat-02:If present, a general practitioner shall at least have a reference, an identifier or a display {generalPractitioner.exists() implies generalPractitioner.all($this.reference.exists() or $this.identifier.exists() or $this.display.exists())}inv-dh-pat-03:If present, a managing organisation shall at least have a reference, an identifier or a display {managingOrganization.exists() implies (managingOrganization.reference.exists() or managingOrganization.identifier.exists() or managingOrganization.display.exists())}</t>
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}inv-pat-0:If there is a birth time its date shall be the birth date {birthDate.extension('http://hl7.org/fhir/StructureDefinition/patient-birthTime').exists() implies birthDate.extension('http://hl7.org/fhir/StructureDefinition/patient-birthTime').value.toString().substring(0,10) = birthDate.toString()}inv-dh-pat-01:One patient name shall have at least a family name {name.family.exists()}inv-dh-pat-02:If present, a general practitioner shall at least have a reference, an identifier or a display {generalPractitioner.exists() implies generalPractitioner.all($this.reference.exists() or $this.identifier.exists() or $this.display.exists())}inv-dh-pat-03:If present, a managing organisation shall at least have a reference, an identifier or a display {managingOrganization.exists() implies (managingOrganization.reference.exists() or managingOrganization.identifier.exists() or managingOrganization.display.exists())}inv-dh-pat-04:If present, date of arrival shall be year of arrival {extension('http://hl7.org.au/fhir/StructureDefinition/date-of-arrival').exists() implies extension.valueDate.value.matches('^([0-9]{4})$')}</t>
   </si>
   <si>
     <t>Patient[classCode=PAT]</t>
@@ -425,7 +425,7 @@
 </t>
   </si>
   <si>
-    <t>The date a person first arrived in Australia, from another country, with the intention of living in Australia for one year or more</t>
+    <t>Year of Arrival</t>
   </si>
   <si>
     <t>The year of arrival in Australia from the Australian Bureau of Statics (ABS) and the Australian Institute of Health and Wealfare (AIHW). The year a person first arrived in Australia, from another country, with the intention of living in Australia for one year or more.</t>
@@ -1587,7 +1587,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-pat-1:SHALL at least contain a contact's details or a reference to an organization {name.exists() or telecom.exists() or address.exists() or organization.exists()}inv-dh-pat-04:If present, a contact's organisation shall at least have a reference, an identifier or a display {organization.exists() implies (organization.reference.exists() or organization.identifier.exists() or organization.display.exists())}</t>
+pat-1:SHALL at least contain a contact's details or a reference to an organization {name.exists() or telecom.exists() or address.exists() or organization.exists()}</t>
   </si>
   <si>
     <t>player[classCode=PSN|ANM and determinerCode=INSTANCE]/scopedRole[classCode=CON]</t>
@@ -1700,10 +1700,6 @@
     <t>Patient.contact.organization</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/organization-dh-base-1)
-</t>
-  </si>
-  <si>
     <t>Organization that is associated with the contact</t>
   </si>
   <si>
@@ -1823,7 +1819,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/organization-dh-base-1|http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/PractitionerRole-dh-base-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/practitionerrole-dh-base-1)
 </t>
   </si>
   <si>
@@ -1845,6 +1841,10 @@
   </si>
   <si>
     <t>Patient.managingOrganization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/organization-dh-base-1)
+</t>
   </si>
   <si>
     <t>Organization that is the custodian of the patient record</t>
@@ -2090,7 +2090,7 @@
     <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="113.41015625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="96.1171875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -3720,7 +3720,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" hidden="true">
+    <row r="15">
       <c r="A15" t="s" s="2">
         <v>95</v>
       </c>
@@ -3738,7 +3738,7 @@
         <v>51</v>
       </c>
       <c r="G15" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="H15" t="s" s="2">
         <v>44</v>
@@ -19740,7 +19740,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="155">
+    <row r="155" hidden="true">
       <c r="A155" t="s" s="2">
         <v>486</v>
       </c>
@@ -19756,7 +19756,7 @@
         <v>43</v>
       </c>
       <c r="G155" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H155" t="s" s="2">
         <v>44</v>
@@ -20198,7 +20198,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="159">
+    <row r="159" hidden="true">
       <c r="A159" t="s" s="2">
         <v>501</v>
       </c>
@@ -20214,7 +20214,7 @@
         <v>43</v>
       </c>
       <c r="G159" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H159" t="s" s="2">
         <v>44</v>
@@ -20312,7 +20312,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="160">
+    <row r="160" hidden="true">
       <c r="A160" t="s" s="2">
         <v>509</v>
       </c>
@@ -20328,7 +20328,7 @@
         <v>51</v>
       </c>
       <c r="G160" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H160" t="s" s="2">
         <v>44</v>
@@ -20426,7 +20426,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="161">
+    <row r="161" hidden="true">
       <c r="A161" t="s" s="2">
         <v>514</v>
       </c>
@@ -20442,7 +20442,7 @@
         <v>43</v>
       </c>
       <c r="G161" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H161" t="s" s="2">
         <v>44</v>
@@ -20542,7 +20542,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="162">
+    <row r="162" hidden="true">
       <c r="A162" t="s" s="2">
         <v>519</v>
       </c>
@@ -20558,7 +20558,7 @@
         <v>51</v>
       </c>
       <c r="G162" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H162" t="s" s="2">
         <v>44</v>
@@ -20656,7 +20656,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="163">
+    <row r="163" hidden="true">
       <c r="A163" t="s" s="2">
         <v>524</v>
       </c>
@@ -20672,7 +20672,7 @@
         <v>51</v>
       </c>
       <c r="G163" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H163" t="s" s="2">
         <v>44</v>
@@ -20770,7 +20770,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="164">
+    <row r="164" hidden="true">
       <c r="A164" t="s" s="2">
         <v>528</v>
       </c>
@@ -20786,7 +20786,7 @@
         <v>51</v>
       </c>
       <c r="G164" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H164" t="s" s="2">
         <v>44</v>
@@ -20795,17 +20795,17 @@
         <v>44</v>
       </c>
       <c r="J164" t="s" s="2">
+        <v>240</v>
+      </c>
+      <c r="K164" t="s" s="2">
         <v>529</v>
       </c>
-      <c r="K164" t="s" s="2">
+      <c r="L164" t="s" s="2">
         <v>530</v>
-      </c>
-      <c r="L164" t="s" s="2">
-        <v>531</v>
       </c>
       <c r="M164" s="2"/>
       <c r="N164" t="s" s="2">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="O164" t="s" s="2">
         <v>44</v>
@@ -20863,13 +20863,13 @@
         <v>51</v>
       </c>
       <c r="AH164" t="s" s="2">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="AI164" t="s" s="2">
         <v>63</v>
       </c>
       <c r="AJ164" t="s" s="2">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="AK164" t="s" s="2">
         <v>158</v>
@@ -20878,15 +20878,15 @@
         <v>44</v>
       </c>
       <c r="AM164" t="s" s="2">
+        <v>534</v>
+      </c>
+      <c r="AN164" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="165" hidden="true">
+      <c r="A165" t="s" s="2">
         <v>535</v>
-      </c>
-      <c r="AN164" t="s" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" t="s" s="2">
-        <v>536</v>
       </c>
       <c r="B165" s="2"/>
       <c r="C165" t="s" s="2">
@@ -20900,7 +20900,7 @@
         <v>51</v>
       </c>
       <c r="G165" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H165" t="s" s="2">
         <v>44</v>
@@ -20912,10 +20912,10 @@
         <v>233</v>
       </c>
       <c r="K165" t="s" s="2">
+        <v>536</v>
+      </c>
+      <c r="L165" t="s" s="2">
         <v>537</v>
-      </c>
-      <c r="L165" t="s" s="2">
-        <v>538</v>
       </c>
       <c r="M165" s="2"/>
       <c r="N165" s="2"/>
@@ -20966,7 +20966,7 @@
         <v>44</v>
       </c>
       <c r="AE165" t="s" s="2">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="AF165" t="s" s="2">
         <v>42</v>
@@ -20981,7 +20981,7 @@
         <v>63</v>
       </c>
       <c r="AJ165" t="s" s="2">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="AK165" t="s" s="2">
         <v>158</v>
@@ -20998,7 +20998,7 @@
     </row>
     <row r="166">
       <c r="A166" t="s" s="2">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B166" s="2"/>
       <c r="C166" t="s" s="2">
@@ -21024,16 +21024,16 @@
         <v>487</v>
       </c>
       <c r="K166" t="s" s="2">
+        <v>540</v>
+      </c>
+      <c r="L166" t="s" s="2">
         <v>541</v>
       </c>
-      <c r="L166" t="s" s="2">
+      <c r="M166" t="s" s="2">
         <v>542</v>
       </c>
-      <c r="M166" t="s" s="2">
+      <c r="N166" t="s" s="2">
         <v>543</v>
-      </c>
-      <c r="N166" t="s" s="2">
-        <v>544</v>
       </c>
       <c r="O166" t="s" s="2">
         <v>44</v>
@@ -21082,7 +21082,7 @@
         <v>44</v>
       </c>
       <c r="AE166" t="s" s="2">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="AF166" t="s" s="2">
         <v>42</v>
@@ -21097,10 +21097,10 @@
         <v>63</v>
       </c>
       <c r="AJ166" t="s" s="2">
+        <v>544</v>
+      </c>
+      <c r="AK166" t="s" s="2">
         <v>545</v>
-      </c>
-      <c r="AK166" t="s" s="2">
-        <v>546</v>
       </c>
       <c r="AL166" t="s" s="2">
         <v>44</v>
@@ -21114,7 +21114,7 @@
     </row>
     <row r="167" hidden="true">
       <c r="A167" t="s" s="2">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B167" s="2"/>
       <c r="C167" t="s" s="2">
@@ -21226,7 +21226,7 @@
     </row>
     <row r="168" hidden="true">
       <c r="A168" t="s" s="2">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B168" s="2"/>
       <c r="C168" t="s" s="2">
@@ -21340,7 +21340,7 @@
     </row>
     <row r="169" hidden="true">
       <c r="A169" t="s" s="2">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B169" s="2"/>
       <c r="C169" t="s" s="2">
@@ -21456,7 +21456,7 @@
     </row>
     <row r="170">
       <c r="A170" t="s" s="2">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B170" s="2"/>
       <c r="C170" t="s" s="2">
@@ -21482,16 +21482,16 @@
         <v>181</v>
       </c>
       <c r="K170" t="s" s="2">
+        <v>550</v>
+      </c>
+      <c r="L170" t="s" s="2">
         <v>551</v>
       </c>
-      <c r="L170" t="s" s="2">
+      <c r="M170" t="s" s="2">
         <v>552</v>
       </c>
-      <c r="M170" t="s" s="2">
+      <c r="N170" t="s" s="2">
         <v>553</v>
-      </c>
-      <c r="N170" t="s" s="2">
-        <v>554</v>
       </c>
       <c r="O170" t="s" s="2">
         <v>44</v>
@@ -21520,7 +21520,7 @@
       </c>
       <c r="X170" s="2"/>
       <c r="Y170" t="s" s="2">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="Z170" t="s" s="2">
         <v>44</v>
@@ -21538,7 +21538,7 @@
         <v>44</v>
       </c>
       <c r="AE170" t="s" s="2">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="AF170" t="s" s="2">
         <v>51</v>
@@ -21553,16 +21553,16 @@
         <v>63</v>
       </c>
       <c r="AJ170" t="s" s="2">
+        <v>555</v>
+      </c>
+      <c r="AK170" t="s" s="2">
         <v>556</v>
       </c>
-      <c r="AK170" t="s" s="2">
+      <c r="AL170" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM170" t="s" s="2">
         <v>557</v>
-      </c>
-      <c r="AL170" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM170" t="s" s="2">
-        <v>558</v>
       </c>
       <c r="AN170" t="s" s="2">
         <v>44</v>
@@ -21570,7 +21570,7 @@
     </row>
     <row r="171">
       <c r="A171" t="s" s="2">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B171" s="2"/>
       <c r="C171" t="s" s="2">
@@ -21596,16 +21596,16 @@
         <v>367</v>
       </c>
       <c r="K171" t="s" s="2">
+        <v>559</v>
+      </c>
+      <c r="L171" t="s" s="2">
         <v>560</v>
       </c>
-      <c r="L171" t="s" s="2">
+      <c r="M171" t="s" s="2">
         <v>561</v>
       </c>
-      <c r="M171" t="s" s="2">
+      <c r="N171" t="s" s="2">
         <v>562</v>
-      </c>
-      <c r="N171" t="s" s="2">
-        <v>563</v>
       </c>
       <c r="O171" t="s" s="2">
         <v>44</v>
@@ -21654,7 +21654,7 @@
         <v>44</v>
       </c>
       <c r="AE171" t="s" s="2">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="AF171" t="s" s="2">
         <v>42</v>
@@ -21669,16 +21669,16 @@
         <v>63</v>
       </c>
       <c r="AJ171" t="s" s="2">
+        <v>563</v>
+      </c>
+      <c r="AK171" t="s" s="2">
         <v>564</v>
       </c>
-      <c r="AK171" t="s" s="2">
+      <c r="AL171" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM171" t="s" s="2">
         <v>565</v>
-      </c>
-      <c r="AL171" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM171" t="s" s="2">
-        <v>566</v>
       </c>
       <c r="AN171" t="s" s="2">
         <v>44</v>
@@ -21686,18 +21686,18 @@
     </row>
     <row r="172">
       <c r="A172" t="s" s="2">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B172" s="2"/>
       <c r="C172" t="s" s="2">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D172" s="2"/>
       <c r="E172" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F172" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="G172" t="s" s="2">
         <v>52</v>
@@ -21709,16 +21709,16 @@
         <v>44</v>
       </c>
       <c r="J172" t="s" s="2">
+        <v>568</v>
+      </c>
+      <c r="K172" t="s" s="2">
         <v>569</v>
       </c>
-      <c r="K172" t="s" s="2">
+      <c r="L172" t="s" s="2">
         <v>570</v>
       </c>
-      <c r="L172" t="s" s="2">
+      <c r="M172" t="s" s="2">
         <v>571</v>
-      </c>
-      <c r="M172" t="s" s="2">
-        <v>572</v>
       </c>
       <c r="N172" s="2"/>
       <c r="O172" t="s" s="2">
@@ -21768,7 +21768,7 @@
         <v>44</v>
       </c>
       <c r="AE172" t="s" s="2">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="AF172" t="s" s="2">
         <v>42</v>
@@ -21783,7 +21783,7 @@
         <v>63</v>
       </c>
       <c r="AJ172" t="s" s="2">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="AK172" t="s" s="2">
         <v>158</v>
@@ -21792,7 +21792,7 @@
         <v>44</v>
       </c>
       <c r="AM172" t="s" s="2">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="AN172" t="s" s="2">
         <v>44</v>
@@ -21800,7 +21800,7 @@
     </row>
     <row r="173">
       <c r="A173" t="s" s="2">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B173" s="2"/>
       <c r="C173" t="s" s="2">
@@ -21823,7 +21823,7 @@
         <v>52</v>
       </c>
       <c r="J173" t="s" s="2">
-        <v>529</v>
+        <v>575</v>
       </c>
       <c r="K173" t="s" s="2">
         <v>576</v>
@@ -21884,7 +21884,7 @@
         <v>44</v>
       </c>
       <c r="AE173" t="s" s="2">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="AF173" t="s" s="2">
         <v>42</v>
@@ -21899,7 +21899,7 @@
         <v>63</v>
       </c>
       <c r="AJ173" t="s" s="2">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="AK173" t="s" s="2">
         <v>580</v>

</xml_diff>

<commit_message>
Changed to My Health Record Patient FHIR profile as of 20210309 Regerated outputs
DR-47
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/patient-mhr-1.xlsx
+++ b/output/DiagnosticReport/patient-mhr-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2390" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2390" uniqueCount="407">
   <si>
     <t>Path</t>
   </si>
@@ -160,7 +160,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}inv-pat-0:If there is a birth time its date shall be the birth date {birthDate.extension('http://hl7.org/fhir/StructureDefinition/patient-birthTime').exists() implies birthDate.extension('http://hl7.org/fhir/StructureDefinition/patient-birthTime').value.toString().substring(0,10) = birthDate.toString()}inv-dh-pat-01:One patient name shall have at least a family name {name.family.exists()}inv-dh-pat-02:If present, a general practitioner shall at least have a reference, an identifier or a display {generalPractitioner.exists() implies generalPractitioner.all($this.reference.exists() or $this.identifier.exists() or $this.display.exists())}inv-dh-pat-03:If present, a managing organisation shall at least have a reference, an identifier or a display {managingOrganization.exists() implies (managingOrganization.reference.exists() or managingOrganization.identifier.exists() or managingOrganization.display.exists())}inv-dh-pat-04:If present, date of arrival shall be year of arrival {extension('http://hl7.org.au/fhir/StructureDefinition/date-of-arrival').exists() implies extension.valueDate.value.matches('^([0-9]{4})$')}</t>
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}inv-pat-0:If there is a birth time its date shall be the birth date {birthDate.extension('http://hl7.org/fhir/StructureDefinition/patient-birthTime').exists() implies birthDate.extension('http://hl7.org/fhir/StructureDefinition/patient-birthTime').value.toString().substring(0,10) = birthDate.toString()}inv-dh-pat-01:The name shall at least have one instance of family name present in family or text {name.family.exists() or name.text.exists()}inv-dh-pat-02:If present, a general practitioner shall at least have a reference, an identifier or a display {generalPractitioner.exists() implies generalPractitioner.all($this.reference.exists() or $this.identifier.exists() or $this.display.exists())}inv-dh-pat-03:If present, date of arrival shall be year of arrival {extension('http://hl7.org.au/fhir/StructureDefinition/date-of-arrival').exists() implies extension.valueDate.value.matches('^([0-9]{4})$')}</t>
   </si>
   <si>
     <t>Patient[classCode=PAT]</t>
@@ -1197,7 +1197,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/practitionerrole-identified-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/practitionerrole-identified-1|http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/organization-identified-1)
 </t>
   </si>
   <si>
@@ -1219,10 +1219,6 @@
   </si>
   <si>
     <t>Patient.managingOrganization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/organization-identified-1)
-</t>
   </si>
   <si>
     <t>Organization that is the custodian of the patient record</t>
@@ -2757,7 +2753,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
         <v>95</v>
       </c>
@@ -2775,7 +2771,7 @@
         <v>51</v>
       </c>
       <c r="G12" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H12" t="s" s="2">
         <v>44</v>
@@ -8154,7 +8150,7 @@
         <v>42</v>
       </c>
       <c r="F59" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G59" t="s" s="2">
         <v>52</v>
@@ -8255,7 +8251,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
         <v>380</v>
       </c>
@@ -8271,7 +8267,7 @@
         <v>51</v>
       </c>
       <c r="G60" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H60" t="s" s="2">
         <v>44</v>
@@ -8280,19 +8276,19 @@
         <v>52</v>
       </c>
       <c r="J60" t="s" s="2">
+        <v>333</v>
+      </c>
+      <c r="K60" t="s" s="2">
         <v>381</v>
       </c>
-      <c r="K60" t="s" s="2">
+      <c r="L60" t="s" s="2">
         <v>382</v>
       </c>
-      <c r="L60" t="s" s="2">
+      <c r="M60" t="s" s="2">
         <v>383</v>
       </c>
-      <c r="M60" t="s" s="2">
+      <c r="N60" t="s" s="2">
         <v>384</v>
-      </c>
-      <c r="N60" t="s" s="2">
-        <v>385</v>
       </c>
       <c r="O60" t="s" s="2">
         <v>44</v>
@@ -8359,7 +8355,7 @@
         <v>338</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="AL60" t="s" s="2">
         <v>44</v>
@@ -8373,7 +8369,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8399,16 +8395,16 @@
         <v>288</v>
       </c>
       <c r="K61" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="L61" t="s" s="2">
         <v>388</v>
       </c>
-      <c r="L61" t="s" s="2">
+      <c r="M61" t="s" s="2">
         <v>389</v>
       </c>
-      <c r="M61" t="s" s="2">
+      <c r="N61" t="s" s="2">
         <v>390</v>
-      </c>
-      <c r="N61" t="s" s="2">
-        <v>391</v>
       </c>
       <c r="O61" t="s" s="2">
         <v>44</v>
@@ -8457,7 +8453,7 @@
         <v>44</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>42</v>
@@ -8472,7 +8468,7 @@
         <v>63</v>
       </c>
       <c r="AJ61" t="s" s="2">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AK61" t="s" s="2">
         <v>169</v>
@@ -8489,7 +8485,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8601,7 +8597,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8715,7 +8711,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8831,7 +8827,7 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -8854,16 +8850,16 @@
         <v>52</v>
       </c>
       <c r="J65" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="K65" t="s" s="2">
         <v>397</v>
       </c>
-      <c r="K65" t="s" s="2">
+      <c r="L65" t="s" s="2">
         <v>398</v>
       </c>
-      <c r="L65" t="s" s="2">
+      <c r="M65" t="s" s="2">
         <v>399</v>
-      </c>
-      <c r="M65" t="s" s="2">
-        <v>400</v>
       </c>
       <c r="N65" s="2"/>
       <c r="O65" t="s" s="2">
@@ -8913,7 +8909,7 @@
         <v>44</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>51</v>
@@ -8928,7 +8924,7 @@
         <v>63</v>
       </c>
       <c r="AJ65" t="s" s="2">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AK65" t="s" s="2">
         <v>169</v>
@@ -8937,7 +8933,7 @@
         <v>44</v>
       </c>
       <c r="AM65" t="s" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AN65" t="s" s="2">
         <v>44</v>
@@ -8945,7 +8941,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -8971,10 +8967,10 @@
         <v>71</v>
       </c>
       <c r="K66" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="L66" t="s" s="2">
         <v>404</v>
-      </c>
-      <c r="L66" t="s" s="2">
-        <v>405</v>
       </c>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
@@ -9004,11 +9000,11 @@
         <v>194</v>
       </c>
       <c r="X66" t="s" s="2">
+        <v>404</v>
+      </c>
+      <c r="Y66" t="s" s="2">
         <v>405</v>
       </c>
-      <c r="Y66" t="s" s="2">
-        <v>406</v>
-      </c>
       <c r="Z66" t="s" s="2">
         <v>44</v>
       </c>
@@ -9025,7 +9021,7 @@
         <v>44</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>51</v>
@@ -9040,7 +9036,7 @@
         <v>63</v>
       </c>
       <c r="AJ66" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="AK66" t="s" s="2">
         <v>169</v>

</xml_diff>